<commit_message>
Script Inicial, creación de BD
</commit_message>
<xml_diff>
--- a/Database/Modelado_BD/Mappeo_tablas_campos.xlsx
+++ b/Database/Modelado_BD/Mappeo_tablas_campos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fjpar\Documents\Dart-Flutter\SaludApp\Database\Modelado_BD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{174A1CF4-CD6E-43CD-8B4E-56B8270EB6A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A7959E-0F7E-4DED-ABCD-F0F0686DAD21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6263086C-BEC1-40A1-A20F-FECA8940B394}"/>
+    <workbookView xWindow="5760" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{6263086C-BEC1-40A1-A20F-FECA8940B394}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,20 +37,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="88">
   <si>
     <t>tb_usuarios</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
     <t>int</t>
   </si>
   <si>
-    <t>nombre</t>
-  </si>
-  <si>
     <t>varchar 100</t>
   </si>
   <si>
@@ -72,9 +66,6 @@
     <t>id_usuario</t>
   </si>
   <si>
-    <t>apellido</t>
-  </si>
-  <si>
     <t>segundo apellido</t>
   </si>
   <si>
@@ -102,9 +93,6 @@
     <t>fecha_actu</t>
   </si>
   <si>
-    <t>rol</t>
-  </si>
-  <si>
     <t>activo</t>
   </si>
   <si>
@@ -120,9 +108,6 @@
     <t>varchar 255</t>
   </si>
   <si>
-    <t>numero_inss</t>
-  </si>
-  <si>
     <t>ocupacion</t>
   </si>
   <si>
@@ -165,7 +150,157 @@
     <t>tb_municipios</t>
   </si>
   <si>
-    <t>ENUM()</t>
+    <t>primer nombre</t>
+  </si>
+  <si>
+    <t>primer apellido</t>
+  </si>
+  <si>
+    <t>numero_inss (solo si tiene)</t>
+  </si>
+  <si>
+    <t>Escolaridad</t>
+  </si>
+  <si>
+    <t>religion</t>
+  </si>
+  <si>
+    <t>persona_emergencia</t>
+  </si>
+  <si>
+    <t>edad</t>
+  </si>
+  <si>
+    <t>estado_civil</t>
+  </si>
+  <si>
+    <t>enum()</t>
+  </si>
+  <si>
+    <t>cantidad_hermanos</t>
+  </si>
+  <si>
+    <t>id_medico</t>
+  </si>
+  <si>
+    <t>egresado_el</t>
+  </si>
+  <si>
+    <t>cod_sanitario</t>
+  </si>
+  <si>
+    <t>especialidad</t>
+  </si>
+  <si>
+    <t>egresado_de</t>
+  </si>
+  <si>
+    <t>experiencia_anyos</t>
+  </si>
+  <si>
+    <t>area_actual</t>
+  </si>
+  <si>
+    <t>centro_actual</t>
+  </si>
+  <si>
+    <t>varchar100</t>
+  </si>
+  <si>
+    <t>tb_ocupaciones</t>
+  </si>
+  <si>
+    <t>tb_religiones</t>
+  </si>
+  <si>
+    <t>id_religion</t>
+  </si>
+  <si>
+    <t>id_departamento</t>
+  </si>
+  <si>
+    <t>id_municipio</t>
+  </si>
+  <si>
+    <t>id_ocupacion</t>
+  </si>
+  <si>
+    <t>tb_passwd</t>
+  </si>
+  <si>
+    <t>id_passwd</t>
+  </si>
+  <si>
+    <t>tb_persona_emergencia</t>
+  </si>
+  <si>
+    <t>id_pemergencia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">segundo nombre </t>
+  </si>
+  <si>
+    <t>varchar  50</t>
+  </si>
+  <si>
+    <t>tb_telefonos</t>
+  </si>
+  <si>
+    <t>id_telefono</t>
+  </si>
+  <si>
+    <t>persona</t>
+  </si>
+  <si>
+    <t>compania</t>
+  </si>
+  <si>
+    <t>tb_prov_telefonicos</t>
+  </si>
+  <si>
+    <t>id_prov_tel</t>
+  </si>
+  <si>
+    <t>proveedor</t>
+  </si>
+  <si>
+    <t>is_user</t>
+  </si>
+  <si>
+    <t>tb_generos</t>
+  </si>
+  <si>
+    <t>id_genero</t>
+  </si>
+  <si>
+    <t>int (campo calculado)</t>
+  </si>
+  <si>
+    <t>turno_actual</t>
+  </si>
+  <si>
+    <t>varchar 9</t>
+  </si>
+  <si>
+    <t>tipo_usuario</t>
+  </si>
+  <si>
+    <t>tb_tipo_usuarios</t>
+  </si>
+  <si>
+    <t>id_tipo_usuario</t>
+  </si>
+  <si>
+    <t>varachar50</t>
+  </si>
+  <si>
+    <t>tb_barrios</t>
+  </si>
+  <si>
+    <t>id_barrio</t>
+  </si>
+  <si>
+    <t>username</t>
   </si>
 </sst>
 </file>
@@ -181,15 +316,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -197,15 +338,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -520,270 +680,614 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1FC444B-680C-45E3-8295-24AB380AFA88}">
-  <dimension ref="B3:I27"/>
+  <dimension ref="B3:M36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5546875" customWidth="1"/>
+    <col min="12" max="12" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="E3" s="1" t="s">
+      <c r="C3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="H3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="2"/>
+      <c r="K3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="L3" s="2"/>
+      <c r="M3" s="3"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M4" s="4"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M5" s="4"/>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="H3" s="1" t="s">
+      <c r="F6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M6" s="4"/>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M7" s="4"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+      <c r="F8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M8" s="4"/>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M9" s="4"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="M10" s="4"/>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M11" s="4"/>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B13" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="L15" s="2"/>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I16" s="2"/>
+      <c r="K16" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B17" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="H17" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="E18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="E19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="H21" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="E22" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" s="2"/>
+      <c r="H22" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
+      <c r="I24" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B27" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="I28" s="2"/>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="E29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B30" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C30" s="2"/>
+      <c r="H30" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B31" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B32" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E33" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" t="s">
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B34" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C34" s="2"/>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B35" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B36" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B21" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="1"/>
-      <c r="E21" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" t="s">
-        <v>2</v>
-      </c>
-      <c r="E22" t="s">
-        <v>1</v>
-      </c>
-      <c r="F22" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23" t="s">
-        <v>35</v>
-      </c>
-      <c r="E23" t="s">
-        <v>31</v>
-      </c>
-      <c r="F23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B25" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25" t="s">
-        <v>32</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B26" t="s">
-        <v>17</v>
-      </c>
-      <c r="C26" t="s">
-        <v>37</v>
-      </c>
-      <c r="E26" t="s">
-        <v>1</v>
-      </c>
-      <c r="F26" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="E27" t="s">
-        <v>33</v>
-      </c>
-      <c r="F27" t="s">
-        <v>32</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="15">
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H28:I28"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="H3:I3"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="E22:F22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>